<commit_message>
Count the Cows G
</commit_message>
<xml_diff>
--- a/usaco-contest/2021Feb/C/CounttheCows.xlsx
+++ b/usaco-contest/2021Feb/C/CounttheCows.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\competitive-programming\usaco-contest\2021Feb\C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\competitive-programming\usaco-contest\2021Feb\C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47469AD-0839-426A-8869-F80A57CDBFC7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E14DC3F-0F43-4E3D-8B31-F9663F8D468A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="37000" windowHeight="18290" activeTab="2" xr2:uid="{A1B670E2-2F1D-420E-859E-64B4349BE0BA}"/>
+    <workbookView xWindow="1395" yWindow="0" windowWidth="37005" windowHeight="18285" activeTab="2" xr2:uid="{A1B670E2-2F1D-420E-859E-64B4349BE0BA}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -299,13 +299,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -375,6 +504,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -396,16 +552,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>108415</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>111509</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>101845</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>118079</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>71244</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>80534</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>64674</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>87104</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -420,8 +576,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="1564269" y="1920485"/>
-          <a:ext cx="1607634" cy="1595244"/>
+          <a:off x="2125086" y="2568303"/>
+          <a:ext cx="1618209" cy="1663818"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -459,10 +615,10 @@
       <xdr:rowOff>83634</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>80537</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114608</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>111673</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>105104</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -477,8 +633,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="250902" y="625707"/>
-          <a:ext cx="1102733" cy="1115121"/>
+          <a:off x="258272" y="648565"/>
+          <a:ext cx="1692711" cy="1716263"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -511,6 +667,63 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>86681</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>113333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>105103</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>164225</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="直接连接符 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC37F029-D781-49A9-B78B-CD8D966E36B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="270612" y="2189126"/>
+          <a:ext cx="4800629" cy="4911927"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="oval" w="med" len="med"/>
+          <a:tailEnd type="oval" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -518,16 +731,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>120650</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>74781</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:rowOff>88756</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>68</xdr:col>
-      <xdr:colOff>146050</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>93</xdr:col>
+      <xdr:colOff>111786</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>117769</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -542,8 +755,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5270500" y="254000"/>
-          <a:ext cx="7391400" cy="7315200"/>
+          <a:off x="2443607" y="279256"/>
+          <a:ext cx="14614396" cy="15045383"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -879,14 +1092,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.4140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="2.4140625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="2.4140625" style="3"/>
+    <col min="1" max="1" width="2.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="2.375" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="2.375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -897,7 +1110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -905,7 +1118,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -913,7 +1126,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
     </row>
-    <row r="4" spans="1:4" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -921,7 +1134,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
     </row>
-    <row r="5" spans="1:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -937,14 +1150,14 @@
       <selection activeCell="E8" sqref="E8:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.4140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="2.4140625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="2.4140625" style="3"/>
+    <col min="1" max="1" width="2.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="2.375" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="2.375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -973,7 +1186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -987,7 +1200,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1001,7 +1214,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1015,7 +1228,7 @@
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
     </row>
-    <row r="5" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1029,7 +1242,7 @@
       <c r="I5" s="15"/>
       <c r="J5" s="16"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1043,7 +1256,7 @@
       <c r="I6" s="18"/>
       <c r="J6" s="19"/>
     </row>
-    <row r="7" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1057,7 +1270,7 @@
       <c r="I7" s="21"/>
       <c r="J7" s="22"/>
     </row>
-    <row r="8" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1071,7 +1284,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1085,7 +1298,7 @@
       <c r="I9" s="8"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1099,7 +1312,7 @@
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1111,18 +1324,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B23B71-1DC1-4023-BDA5-AF5388257871}">
   <dimension ref="A1:AB29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:G10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.4140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="28" width="2.4140625" style="3" customWidth="1"/>
-    <col min="29" max="16384" width="2.4140625" style="3"/>
+    <col min="1" max="1" width="2.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="28" width="2.375" style="3" customWidth="1"/>
+    <col min="29" max="16384" width="2.375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -1205,7 +1418,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1237,7 +1450,7 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="6"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1269,7 +1482,7 @@
       <c r="AA3" s="8"/>
       <c r="AB3" s="9"/>
     </row>
-    <row r="4" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1301,7 +1514,7 @@
       <c r="AA4" s="12"/>
       <c r="AB4" s="13"/>
     </row>
-    <row r="5" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1333,7 +1546,7 @@
       <c r="AA5" s="15"/>
       <c r="AB5" s="16"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1365,7 +1578,7 @@
       <c r="AA6" s="18"/>
       <c r="AB6" s="19"/>
     </row>
-    <row r="7" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1397,7 +1610,7 @@
       <c r="AA7" s="21"/>
       <c r="AB7" s="22"/>
     </row>
-    <row r="8" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1429,7 +1642,7 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="6"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1461,7 +1674,7 @@
       <c r="AA9" s="8"/>
       <c r="AB9" s="9"/>
     </row>
-    <row r="10" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1493,7 +1706,7 @@
       <c r="AA10" s="12"/>
       <c r="AB10" s="13"/>
     </row>
-    <row r="11" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1525,7 +1738,7 @@
       <c r="AA11" s="15"/>
       <c r="AB11" s="16"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1557,7 +1770,7 @@
       <c r="AA12" s="18"/>
       <c r="AB12" s="19"/>
     </row>
-    <row r="13" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1589,7 +1802,7 @@
       <c r="AA13" s="18"/>
       <c r="AB13" s="19"/>
     </row>
-    <row r="14" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1621,7 +1834,7 @@
       <c r="AA14" s="18"/>
       <c r="AB14" s="19"/>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1653,7 +1866,7 @@
       <c r="AA15" s="18"/>
       <c r="AB15" s="19"/>
     </row>
-    <row r="16" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1685,7 +1898,7 @@
       <c r="AA16" s="18"/>
       <c r="AB16" s="19"/>
     </row>
-    <row r="17" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1717,7 +1930,7 @@
       <c r="AA17" s="18"/>
       <c r="AB17" s="19"/>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1749,7 +1962,7 @@
       <c r="AA18" s="18"/>
       <c r="AB18" s="19"/>
     </row>
-    <row r="19" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1781,7 +1994,7 @@
       <c r="AA19" s="21"/>
       <c r="AB19" s="22"/>
     </row>
-    <row r="20" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1813,7 +2026,7 @@
       <c r="AA20" s="5"/>
       <c r="AB20" s="6"/>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1845,7 +2058,7 @@
       <c r="AA21" s="8"/>
       <c r="AB21" s="9"/>
     </row>
-    <row r="22" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1877,7 +2090,7 @@
       <c r="AA22" s="12"/>
       <c r="AB22" s="13"/>
     </row>
-    <row r="23" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1909,7 +2122,7 @@
       <c r="AA23" s="15"/>
       <c r="AB23" s="16"/>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1941,7 +2154,7 @@
       <c r="AA24" s="18"/>
       <c r="AB24" s="19"/>
     </row>
-    <row r="25" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1973,7 +2186,7 @@
       <c r="AA25" s="21"/>
       <c r="AB25" s="22"/>
     </row>
-    <row r="26" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2005,7 +2218,7 @@
       <c r="AA26" s="5"/>
       <c r="AB26" s="6"/>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2037,7 +2250,7 @@
       <c r="AA27" s="8"/>
       <c r="AB27" s="9"/>
     </row>
-    <row r="28" spans="1:28" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2069,7 +2282,7 @@
       <c r="AA28" s="12"/>
       <c r="AB28" s="13"/>
     </row>
-    <row r="29" spans="1:28" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:28" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2082,18 +2295,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C05293-E3D8-4203-82C9-78D7D943FDD4}">
   <dimension ref="A1:CD83"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="BO34" sqref="BO34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.4140625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="2.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="28" width="2.4140625" style="3" customWidth="1"/>
-    <col min="29" max="16384" width="2.4140625" style="3"/>
+    <col min="1" max="1" width="2.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="28" width="2.375" style="3" customWidth="1"/>
+    <col min="29" max="16384" width="2.375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>0</v>
       </c>
@@ -2338,7 +2551,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2351,6 +2564,15 @@
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="25"/>
       <c r="T2" s="4"/>
       <c r="U2" s="5"/>
       <c r="V2" s="6"/>
@@ -2379,7 +2601,7 @@
       <c r="CC2" s="5"/>
       <c r="CD2" s="6"/>
     </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2392,6 +2614,15 @@
       <c r="H3" s="7"/>
       <c r="I3" s="8"/>
       <c r="J3" s="9"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="28"/>
       <c r="T3" s="7"/>
       <c r="U3" s="8"/>
       <c r="V3" s="9"/>
@@ -2420,7 +2651,7 @@
       <c r="CC3" s="8"/>
       <c r="CD3" s="9"/>
     </row>
-    <row r="4" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2433,6 +2664,15 @@
       <c r="H4" s="11"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="28"/>
       <c r="T4" s="11"/>
       <c r="U4" s="12"/>
       <c r="V4" s="13"/>
@@ -2461,7 +2701,7 @@
       <c r="CC4" s="12"/>
       <c r="CD4" s="13"/>
     </row>
-    <row r="5" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2474,6 +2714,15 @@
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="28"/>
       <c r="T5" s="7"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
@@ -2502,7 +2751,7 @@
       <c r="CC5" s="10"/>
       <c r="CD5" s="9"/>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2515,6 +2764,15 @@
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="9"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
       <c r="T6" s="7"/>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
@@ -2543,7 +2801,7 @@
       <c r="CC6" s="10"/>
       <c r="CD6" s="9"/>
     </row>
-    <row r="7" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2556,6 +2814,15 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="J7" s="9"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="28"/>
       <c r="T7" s="7"/>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
@@ -2584,7 +2851,7 @@
       <c r="CC7" s="10"/>
       <c r="CD7" s="9"/>
     </row>
-    <row r="8" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2597,6 +2864,15 @@
       <c r="H8" s="4"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="28"/>
       <c r="T8" s="4"/>
       <c r="U8" s="5"/>
       <c r="V8" s="6"/>
@@ -2625,7 +2901,7 @@
       <c r="CC8" s="5"/>
       <c r="CD8" s="6"/>
     </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2638,6 +2914,15 @@
       <c r="H9" s="7"/>
       <c r="I9" s="8"/>
       <c r="J9" s="9"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="28"/>
       <c r="T9" s="7"/>
       <c r="U9" s="8"/>
       <c r="V9" s="9"/>
@@ -2666,7 +2951,7 @@
       <c r="CC9" s="8"/>
       <c r="CD9" s="9"/>
     </row>
-    <row r="10" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2679,6 +2964,15 @@
       <c r="H10" s="11"/>
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="31"/>
       <c r="T10" s="11"/>
       <c r="U10" s="12"/>
       <c r="V10" s="13"/>
@@ -2707,7 +3001,7 @@
       <c r="CC10" s="12"/>
       <c r="CD10" s="13"/>
     </row>
-    <row r="11" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2730,7 +3024,7 @@
       <c r="BT11" s="5"/>
       <c r="BU11" s="6"/>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2753,7 +3047,7 @@
       <c r="BT12" s="8"/>
       <c r="BU12" s="9"/>
     </row>
-    <row r="13" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2776,7 +3070,7 @@
       <c r="BT13" s="12"/>
       <c r="BU13" s="13"/>
     </row>
-    <row r="14" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2799,7 +3093,7 @@
       <c r="BT14" s="10"/>
       <c r="BU14" s="9"/>
     </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2822,7 +3116,7 @@
       <c r="BT15" s="10"/>
       <c r="BU15" s="9"/>
     </row>
-    <row r="16" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2845,7 +3139,7 @@
       <c r="BT16" s="10"/>
       <c r="BU16" s="9"/>
     </row>
-    <row r="17" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2868,7 +3162,7 @@
       <c r="BT17" s="5"/>
       <c r="BU17" s="6"/>
     </row>
-    <row r="18" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2891,7 +3185,7 @@
       <c r="BT18" s="8"/>
       <c r="BU18" s="9"/>
     </row>
-    <row r="19" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2914,7 +3208,7 @@
       <c r="BT19" s="12"/>
       <c r="BU19" s="13"/>
     </row>
-    <row r="20" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2955,7 +3249,7 @@
       <c r="CC20" s="5"/>
       <c r="CD20" s="6"/>
     </row>
-    <row r="21" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2996,7 +3290,7 @@
       <c r="CC21" s="8"/>
       <c r="CD21" s="9"/>
     </row>
-    <row r="22" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3037,7 +3331,7 @@
       <c r="CC22" s="12"/>
       <c r="CD22" s="13"/>
     </row>
-    <row r="23" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -3078,7 +3372,7 @@
       <c r="CC23" s="10"/>
       <c r="CD23" s="9"/>
     </row>
-    <row r="24" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -3119,7 +3413,7 @@
       <c r="CC24" s="10"/>
       <c r="CD24" s="9"/>
     </row>
-    <row r="25" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3160,7 +3454,7 @@
       <c r="CC25" s="10"/>
       <c r="CD25" s="9"/>
     </row>
-    <row r="26" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3201,7 +3495,7 @@
       <c r="CC26" s="5"/>
       <c r="CD26" s="6"/>
     </row>
-    <row r="27" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -3242,7 +3536,7 @@
       <c r="CC27" s="8"/>
       <c r="CD27" s="9"/>
     </row>
-    <row r="28" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -3283,7 +3577,7 @@
       <c r="CC28" s="12"/>
       <c r="CD28" s="13"/>
     </row>
-    <row r="29" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -3306,7 +3600,7 @@
       <c r="BB29" s="5"/>
       <c r="BC29" s="6"/>
     </row>
-    <row r="30" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -3329,7 +3623,7 @@
       <c r="BB30" s="8"/>
       <c r="BC30" s="9"/>
     </row>
-    <row r="31" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3352,7 +3646,7 @@
       <c r="BB31" s="12"/>
       <c r="BC31" s="13"/>
     </row>
-    <row r="32" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3375,7 +3669,7 @@
       <c r="BB32" s="10"/>
       <c r="BC32" s="9"/>
     </row>
-    <row r="33" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3398,7 +3692,7 @@
       <c r="BB33" s="10"/>
       <c r="BC33" s="9"/>
     </row>
-    <row r="34" spans="1:55" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3421,7 +3715,7 @@
       <c r="BB34" s="10"/>
       <c r="BC34" s="9"/>
     </row>
-    <row r="35" spans="1:55" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:55" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3444,7 +3738,7 @@
       <c r="BB35" s="5"/>
       <c r="BC35" s="6"/>
     </row>
-    <row r="36" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3467,7 +3761,7 @@
       <c r="BB36" s="8"/>
       <c r="BC36" s="9"/>
     </row>
-    <row r="37" spans="1:55" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3490,7 +3784,7 @@
       <c r="BB37" s="12"/>
       <c r="BC37" s="13"/>
     </row>
-    <row r="38" spans="1:55" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:55" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3504,7 +3798,7 @@
       <c r="AS38" s="5"/>
       <c r="AT38" s="6"/>
     </row>
-    <row r="39" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3518,7 +3812,7 @@
       <c r="AS39" s="8"/>
       <c r="AT39" s="9"/>
     </row>
-    <row r="40" spans="1:55" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3532,7 +3826,7 @@
       <c r="AS40" s="12"/>
       <c r="AT40" s="13"/>
     </row>
-    <row r="41" spans="1:55" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:55" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3546,7 +3840,7 @@
       <c r="AS41" s="10"/>
       <c r="AT41" s="9"/>
     </row>
-    <row r="42" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3560,7 +3854,7 @@
       <c r="AS42" s="10"/>
       <c r="AT42" s="9"/>
     </row>
-    <row r="43" spans="1:55" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3574,7 +3868,7 @@
       <c r="AS43" s="10"/>
       <c r="AT43" s="9"/>
     </row>
-    <row r="44" spans="1:55" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:55" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3588,7 +3882,7 @@
       <c r="AS44" s="5"/>
       <c r="AT44" s="6"/>
     </row>
-    <row r="45" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3602,7 +3896,7 @@
       <c r="AS45" s="8"/>
       <c r="AT45" s="9"/>
     </row>
-    <row r="46" spans="1:55" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3616,7 +3910,7 @@
       <c r="AS46" s="12"/>
       <c r="AT46" s="13"/>
     </row>
-    <row r="47" spans="1:55" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:55" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3639,7 +3933,7 @@
       <c r="BB47" s="5"/>
       <c r="BC47" s="6"/>
     </row>
-    <row r="48" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3662,7 +3956,7 @@
       <c r="BB48" s="8"/>
       <c r="BC48" s="9"/>
     </row>
-    <row r="49" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3685,7 +3979,7 @@
       <c r="BB49" s="12"/>
       <c r="BC49" s="13"/>
     </row>
-    <row r="50" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3708,7 +4002,7 @@
       <c r="BB50" s="10"/>
       <c r="BC50" s="9"/>
     </row>
-    <row r="51" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3731,7 +4025,7 @@
       <c r="BB51" s="10"/>
       <c r="BC51" s="9"/>
     </row>
-    <row r="52" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3754,7 +4048,7 @@
       <c r="BB52" s="10"/>
       <c r="BC52" s="9"/>
     </row>
-    <row r="53" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3777,7 +4071,7 @@
       <c r="BB53" s="5"/>
       <c r="BC53" s="6"/>
     </row>
-    <row r="54" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3800,7 +4094,7 @@
       <c r="BB54" s="8"/>
       <c r="BC54" s="9"/>
     </row>
-    <row r="55" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -3823,7 +4117,7 @@
       <c r="BB55" s="12"/>
       <c r="BC55" s="13"/>
     </row>
-    <row r="56" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -3864,7 +4158,7 @@
       <c r="CC56" s="5"/>
       <c r="CD56" s="6"/>
     </row>
-    <row r="57" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -3905,7 +4199,7 @@
       <c r="CC57" s="8"/>
       <c r="CD57" s="9"/>
     </row>
-    <row r="58" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -3946,7 +4240,7 @@
       <c r="CC58" s="12"/>
       <c r="CD58" s="13"/>
     </row>
-    <row r="59" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3987,7 +4281,7 @@
       <c r="CC59" s="10"/>
       <c r="CD59" s="9"/>
     </row>
-    <row r="60" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4028,7 +4322,7 @@
       <c r="CC60" s="10"/>
       <c r="CD60" s="9"/>
     </row>
-    <row r="61" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4069,7 +4363,7 @@
       <c r="CC61" s="10"/>
       <c r="CD61" s="9"/>
     </row>
-    <row r="62" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4110,7 +4404,7 @@
       <c r="CC62" s="5"/>
       <c r="CD62" s="6"/>
     </row>
-    <row r="63" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4151,7 +4445,7 @@
       <c r="CC63" s="8"/>
       <c r="CD63" s="9"/>
     </row>
-    <row r="64" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4192,7 +4486,7 @@
       <c r="CC64" s="12"/>
       <c r="CD64" s="13"/>
     </row>
-    <row r="65" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4215,7 +4509,7 @@
       <c r="BT65" s="5"/>
       <c r="BU65" s="6"/>
     </row>
-    <row r="66" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4238,7 +4532,7 @@
       <c r="BT66" s="8"/>
       <c r="BU66" s="9"/>
     </row>
-    <row r="67" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4261,7 +4555,7 @@
       <c r="BT67" s="12"/>
       <c r="BU67" s="13"/>
     </row>
-    <row r="68" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4284,7 +4578,7 @@
       <c r="BT68" s="10"/>
       <c r="BU68" s="9"/>
     </row>
-    <row r="69" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4307,7 +4601,7 @@
       <c r="BT69" s="10"/>
       <c r="BU69" s="9"/>
     </row>
-    <row r="70" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4330,7 +4624,7 @@
       <c r="BT70" s="10"/>
       <c r="BU70" s="9"/>
     </row>
-    <row r="71" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4353,7 +4647,7 @@
       <c r="BT71" s="5"/>
       <c r="BU71" s="6"/>
     </row>
-    <row r="72" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4376,7 +4670,7 @@
       <c r="BT72" s="8"/>
       <c r="BU72" s="9"/>
     </row>
-    <row r="73" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4399,7 +4693,7 @@
       <c r="BT73" s="12"/>
       <c r="BU73" s="13"/>
     </row>
-    <row r="74" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4440,7 +4734,7 @@
       <c r="CC74" s="5"/>
       <c r="CD74" s="6"/>
     </row>
-    <row r="75" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -4481,7 +4775,7 @@
       <c r="CC75" s="8"/>
       <c r="CD75" s="9"/>
     </row>
-    <row r="76" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -4522,7 +4816,7 @@
       <c r="CC76" s="12"/>
       <c r="CD76" s="13"/>
     </row>
-    <row r="77" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -4563,7 +4857,7 @@
       <c r="CC77" s="10"/>
       <c r="CD77" s="9"/>
     </row>
-    <row r="78" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -4604,7 +4898,7 @@
       <c r="CC78" s="10"/>
       <c r="CD78" s="9"/>
     </row>
-    <row r="79" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -4645,7 +4939,7 @@
       <c r="CC79" s="10"/>
       <c r="CD79" s="9"/>
     </row>
-    <row r="80" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -4686,7 +4980,7 @@
       <c r="CC80" s="5"/>
       <c r="CD80" s="6"/>
     </row>
-    <row r="81" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -4727,7 +5021,7 @@
       <c r="CC81" s="8"/>
       <c r="CD81" s="9"/>
     </row>
-    <row r="82" spans="1:82" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -4768,11 +5062,11 @@
       <c r="CC82" s="12"/>
       <c r="CD82" s="13"/>
     </row>
-    <row r="83" spans="1:82" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:82" ht="15" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" copies="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>